<commit_message>
removed dependency on desktop-based csv file for testing
</commit_message>
<xml_diff>
--- a/src/test/resources/files/test.xlsx
+++ b/src/test/resources/files/test.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,26 +20,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Project Name</t>
   </si>
   <si>
     <t xml:space="preserve">Useless Project</t>
   </si>
+  <si>
+    <t xml:space="preserve">Project Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Age (Years)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miscellaneous Issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a longish string that needs to be handled by the program. You cannot underestimate how important this is.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -99,8 +113,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -121,15 +139,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -138,6 +158,30 @@
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>42027</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>